<commit_message>
add things 	new file:   exp11/data/fits_ar_1.nb 	new file:   exp11/data/fits_ar_2.nb 	renamed:    exp11/data/fits.nb -> exp11/data/fits_co2_1.nb 	new file:   exp11/data/fits_co2_2.nb 	new file:   exp11/data/fits_n_1.nb 	new file:   exp11/data/fits_n_2.nb 	modified:   exp11/data/oscillations.xlsx 	modified:   exp11/data/readings.xlsx
</commit_message>
<xml_diff>
--- a/exp11/data/oscillations.xlsx
+++ b/exp11/data/oscillations.xlsx
@@ -170,10 +170,10 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -366,11 +366,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86333141"/>
-        <c:axId val="84261474"/>
+        <c:axId val="27595485"/>
+        <c:axId val="35073392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86333141"/>
+        <c:axId val="27595485"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84261474"/>
+        <c:crossAx val="35073392"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -389,7 +389,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84261474"/>
+        <c:axId val="35073392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86333141"/>
+        <c:crossAx val="27595485"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -451,7 +451,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
           </c:spPr>
           <c:marker/>
@@ -618,11 +618,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="28671094"/>
-        <c:axId val="42338189"/>
+        <c:axId val="64416171"/>
+        <c:axId val="94366507"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28671094"/>
+        <c:axId val="64416171"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,8 +630,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42338189"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="94366507"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -641,7 +641,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42338189"/>
+        <c:axId val="94366507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,8 +658,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="28671094"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="64416171"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -703,7 +703,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff420e"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
           </c:spPr>
           <c:marker/>
@@ -759,50 +759,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>13.2559728</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3458456</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9357184</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5255912</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.615464</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7053368</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7952096</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3850824</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9749552</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.064828</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1547008</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.28092800011359E-005</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="37842828"/>
-        <c:axId val="89137642"/>
+        <c:axId val="58741297"/>
+        <c:axId val="28641123"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37842828"/>
+        <c:axId val="58741297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,8 +810,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89137642"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="28641123"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -821,7 +821,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89137642"/>
+        <c:axId val="28641123"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,8 +838,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37842828"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="58741297"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -875,15 +875,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>310680</xdr:colOff>
+      <xdr:colOff>337680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:colOff>407160</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -891,8 +891,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7625880" y="1909080"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="7652880" y="1900080"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -905,15 +905,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>304560</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>346680</xdr:colOff>
+      <xdr:colOff>373320</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -921,8 +921,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4341240" y="8114760"/>
-        <a:ext cx="5758920" cy="3240360"/>
+        <a:off x="4368240" y="8105760"/>
+        <a:ext cx="5758560" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -935,15 +935,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
+      <xdr:colOff>245520</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>287640</xdr:colOff>
+      <xdr:colOff>314280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -951,8 +951,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8346240" y="6201720"/>
-        <a:ext cx="5758920" cy="3240000"/>
+        <a:off x="8373240" y="6192720"/>
+        <a:ext cx="5758560" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -970,10 +970,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K46" activeCellId="0" pane="topLeft" sqref="K46"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E40" activeCellId="0" pane="topLeft" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1547,6 +1547,10 @@
       <c r="J37" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="K37" s="0" t="n">
+        <f aca="false">MIN(H38:H49)</f>
+        <v>19.83391280928</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">

</xml_diff>